<commit_message>
Actualización de archivos JSON y scripts 17 de octubre
</commit_message>
<xml_diff>
--- a/Colpatria.xlsx
+++ b/Colpatria.xlsx
@@ -96,10 +96,11 @@
     <t>Se requiere crear un clasificador de documentos para el proceso de afiliaciones</t>
   </si>
   <si>
-    <t>EN PROCESO</t>
+    <t>PAUSADO</t>
   </si>
   <si>
-    <t>Se tiene ya construida la base del entranamiento</t>
+    <t>Se tiene ya construida la base del entranamiento
+15/10/2025: Se Pausa este requerimiento mientras se avanza en otras automatizaciones del proceso de afiliaciones</t>
   </si>
   <si>
     <t>COLP25-0002</t>
@@ -113,11 +114,11 @@
 - Ajustar el proceso diario de preparación de archivos
 - Ajustar visualización de imagenes posterior a generar lotes
 - Ajustar para que se mantengan los filtros del gestor lote
-- Permitir carga de otros tipos de archivos (xlsx, correos, word o zip)
+- Permitir carga de otros tipos de archivos (xlsx, correos, word)
 - Los excel NR, no salen completos, ajustar el pantallazo al tamaño de la tabla</t>
   </si>
   <si>
-    <t>PASO A PRODUCCION</t>
+    <t>FINALIZADO</t>
   </si>
   <si>
     <t>12/09/2025: Se ajusta la resolucion de imagenes
@@ -135,6 +136,9 @@
     <t>El informe de usuarios de Imagine se envia de forma mensual, en los primeros 5 dias del mes, este proceso realiza de forma manual y se requiere habilitar un proceso automatico para que lo envie</t>
   </si>
   <si>
+    <t>EN PROCESO</t>
+  </si>
+  <si>
     <t>03/10/2025: Se revisa el proceso de la generación del informe con John
 03/10/2025: Se realizaron ajustes en el reporte, se corregen inconsistencias que se ajustadas de forma manual actualmente</t>
   </si>
@@ -146,6 +150,9 @@
   </si>
   <si>
     <t>Se requiere una opcion que permite agilizar el proceso de alistamiento del archivo de nomina, ya que es algo que quita mucho tiempo por cada archivo</t>
+  </si>
+  <si>
+    <t>PASO A PRODUCCION</t>
   </si>
   <si>
     <t xml:space="preserve">22/08/2025: Se crea la estructura y la lectura del archivo, se mapean algunos campos del excel
@@ -164,9 +171,6 @@
   </si>
   <si>
     <t>Este desarrollo es para reducir la manuallidad de procesar archivos de excel de forma manual, este permitir realizar las trasnformaciones de los valores de las columnas y validar la información</t>
-  </si>
-  <si>
-    <t>PAUSADO</t>
   </si>
   <si>
     <t>22/08/2025: Se han agregado mejoras y optimizaciones al proceso de transformación del archivo masivo
@@ -259,9 +263,6 @@
   </si>
   <si>
     <t>Implementación de cartas (Devolución, glosa y pago).</t>
-  </si>
-  <si>
-    <t>FINALIZADO</t>
   </si>
   <si>
     <t>*02/10/2024 ya se encuentra implementado</t>
@@ -624,7 +625,7 @@
     <t>Internal Server Error</t>
   </si>
   <si>
-    <t>TRUE</t>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -2190,8 +2191,8 @@
   <dimension ref="A1:AM940"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2212,7 +2213,7 @@
     <col min="14" max="14" width="11" customWidth="1"/>
     <col min="15" max="15" width="17.21875" customWidth="1"/>
     <col min="16" max="16" width="33.44140625" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
     <col min="18" max="39" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2322,7 +2323,7 @@
       <c r="L2" s="25"/>
       <c r="M2" s="26">
         <f ca="1">IF(ISBLANK(L2), NETWORKDAYS(J2, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J2, L2, Hoja2!$A$1:$A$18))</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
@@ -2355,7 +2356,7 @@
       <c r="AL2" s="13"/>
       <c r="AM2" s="13"/>
     </row>
-    <row r="3" spans="1:39" ht="53.25" customHeight="1">
+    <row r="3" spans="1:39" ht="178.5">
       <c r="A3" s="14" t="s">
         <v>17</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>26</v>
       </c>
       <c r="G3" s="20">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="H3" s="21"/>
       <c r="I3" s="29"/>
@@ -2383,10 +2384,12 @@
       <c r="K3" s="30">
         <v>45947</v>
       </c>
-      <c r="L3" s="25"/>
+      <c r="L3" s="30">
+        <v>45945</v>
+      </c>
       <c r="M3" s="26">
         <f ca="1">IF(ISBLANK(L3), NETWORKDAYS(J3, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J3, L3, Hoja2!$A$1:$A$18))</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N3" s="31"/>
       <c r="O3" s="32"/>
@@ -2434,7 +2437,7 @@
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="19" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G4" s="20">
         <v>80</v>
@@ -2450,12 +2453,12 @@
       <c r="L4" s="25"/>
       <c r="M4" s="26">
         <f ca="1">IF(ISBLANK(L4), NETWORKDAYS(J4, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J4, L4, Hoja2!$A$1:$A$18))</f>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="N4" s="25"/>
       <c r="O4" s="32"/>
       <c r="P4" s="33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="28" t="s">
         <v>155</v>
@@ -2488,17 +2491,17 @@
         <v>17</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="19" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G5" s="20">
         <v>90</v>
@@ -2514,7 +2517,7 @@
       <c r="L5" s="25"/>
       <c r="M5" s="26">
         <f ca="1">IF(ISBLANK(L5), NETWORKDAYS(J5, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J5, L5, Hoja2!$A$1:$A$18))</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N5" s="30">
         <v>45909</v>
@@ -2523,7 +2526,7 @@
         <v>45919</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Q5" s="28" t="s">
         <v>155</v>
@@ -2556,17 +2559,17 @@
         <v>17</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="19" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G6" s="20">
         <v>90</v>
@@ -2582,12 +2585,12 @@
       <c r="L6" s="36"/>
       <c r="M6" s="26">
         <f ca="1">IF(ISBLANK(L6), NETWORKDAYS(J6, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J6, L6, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
       <c r="P6" s="27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q6" s="28" t="s">
         <v>155</v>
@@ -2620,17 +2623,17 @@
         <v>17</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="19" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G7" s="20">
         <v>97</v>
@@ -2646,12 +2649,12 @@
       <c r="L7" s="36"/>
       <c r="M7" s="26">
         <f ca="1">IF(ISBLANK(L7), NETWORKDAYS(J7, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J7, L7, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N7" s="37"/>
       <c r="O7" s="38"/>
       <c r="P7" s="33" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="28" t="s">
         <v>155</v>
@@ -2684,17 +2687,17 @@
         <v>17</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="19" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G8" s="20">
         <v>90</v>
@@ -2710,12 +2713,12 @@
       <c r="L8" s="25"/>
       <c r="M8" s="26">
         <f ca="1">IF(ISBLANK(L8), NETWORKDAYS(J8, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J8, L8, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N8" s="25"/>
       <c r="O8" s="38"/>
       <c r="P8" s="33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q8" s="28" t="s">
         <v>155</v>
@@ -2748,17 +2751,17 @@
         <v>17</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G9" s="20">
         <v>0</v>
@@ -2774,12 +2777,12 @@
       <c r="L9" s="25"/>
       <c r="M9" s="26">
         <f ca="1">IF(ISBLANK(L9), NETWORKDAYS(J9, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J9, L9, Hoja2!$A$1:$A$18))</f>
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="N9" s="25"/>
       <c r="O9" s="38"/>
       <c r="P9" s="33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q9" s="28" t="s">
         <v>155</v>
@@ -2822,7 +2825,7 @@
       <c r="L10" s="29"/>
       <c r="M10" s="26">
         <f ca="1">IF(ISBLANK(L10), NETWORKDAYS(J10, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J10, L10, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N10" s="37"/>
       <c r="O10" s="38"/>
@@ -2866,7 +2869,7 @@
       <c r="L11" s="25"/>
       <c r="M11" s="26">
         <f ca="1">IF(ISBLANK(L11), NETWORKDAYS(J11, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J11, L11, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="38"/>
@@ -2910,7 +2913,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26">
         <f ca="1">IF(ISBLANK(L12), NETWORKDAYS(J12, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J12, L12, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="38"/>
@@ -2954,7 +2957,7 @@
       <c r="L13" s="25"/>
       <c r="M13" s="26">
         <f ca="1">IF(ISBLANK(L13), NETWORKDAYS(J13, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J13, L13, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="38"/>
@@ -2998,7 +3001,7 @@
       <c r="L14" s="25"/>
       <c r="M14" s="26">
         <f ca="1">IF(ISBLANK(L14), NETWORKDAYS(J14, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J14, L14, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N14" s="25"/>
       <c r="O14" s="38"/>
@@ -3042,7 +3045,7 @@
       <c r="L15" s="25"/>
       <c r="M15" s="26">
         <f ca="1">IF(ISBLANK(L15), NETWORKDAYS(J15, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J15, L15, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N15" s="25"/>
       <c r="O15" s="38"/>
@@ -3086,7 +3089,7 @@
       <c r="L16" s="25"/>
       <c r="M16" s="26">
         <f ca="1">IF(ISBLANK(L16), NETWORKDAYS(J16, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J16, L16, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N16" s="25"/>
       <c r="O16" s="38"/>
@@ -3130,7 +3133,7 @@
       <c r="L17" s="36"/>
       <c r="M17" s="26">
         <f ca="1">IF(ISBLANK(L17), NETWORKDAYS(J17, TODAY(),Hoja2!$A$1:$A$18), NETWORKDAYS(J17, L17, Hoja2!$A$1:$A$18))</f>
-        <v>32795</v>
+        <v>32802</v>
       </c>
       <c r="N17" s="37"/>
       <c r="O17" s="38"/>
@@ -41052,7 +41055,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="30">
       <c r="A1" s="108" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B1" s="108" t="s">
         <v>2</v>
@@ -41073,19 +41076,19 @@
         <v>10</v>
       </c>
       <c r="H1" s="109" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I1" s="109" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="111" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K1" s="108" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L1" s="112" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M1" s="113"/>
       <c r="N1" s="113"/>
@@ -41104,14 +41107,14 @@
     </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" s="114" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" s="115" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="116"/>
       <c r="D2" s="117" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E2" s="118">
         <v>45526</v>
@@ -41125,7 +41128,7 @@
       <c r="J2" s="116"/>
       <c r="K2" s="116"/>
       <c r="L2" s="116" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="M2" s="119"/>
       <c r="N2" s="119"/>
@@ -41144,16 +41147,16 @@
     </row>
     <row r="3" spans="1:26" ht="28.5">
       <c r="A3" s="120" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="121" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3" s="122" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3" s="122" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="E3" s="123">
         <v>45560</v>
@@ -41244,7 +41247,7 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="112" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="128" t="s">
         <v>72</v>
@@ -41342,10 +41345,10 @@
     </row>
     <row r="7" spans="1:26" ht="99.75">
       <c r="A7" s="112" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="121" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="140" t="s">
         <v>81</v>
@@ -41391,7 +41394,7 @@
     </row>
     <row r="8" spans="1:26" ht="71.25">
       <c r="A8" s="144" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="145" t="s">
         <v>83</v>
@@ -50087,7 +50090,7 @@
     </row>
     <row r="5" spans="1:97" ht="15.75" customHeight="1">
       <c r="A5" s="167" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="168" t="s">
         <v>122</v>
@@ -53371,7 +53374,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5">
       <c r="A1" s="174" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B1" s="174" t="s">
         <v>2</v>
@@ -53392,19 +53395,19 @@
         <v>10</v>
       </c>
       <c r="H1" s="175" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I1" s="177" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="178" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K1" s="179" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L1" s="177" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M1" s="180"/>
       <c r="N1" s="180"/>
@@ -53430,7 +53433,7 @@
       </c>
       <c r="C2" s="183"/>
       <c r="D2" s="183" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="E2" s="184">
         <v>45567</v>
@@ -53481,7 +53484,7 @@
         <v>149</v>
       </c>
       <c r="D3" s="183" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E3" s="184">
         <v>45575</v>
@@ -53526,7 +53529,7 @@
         <v>151</v>
       </c>
       <c r="D4" s="183" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="184">
         <v>45575</v>
@@ -53573,7 +53576,7 @@
         <v>154</v>
       </c>
       <c r="D5" s="183" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" s="184">
         <v>45575</v>

</xml_diff>

<commit_message>
Actualización de archivos JSON y scripts 25  de febrero 2026
</commit_message>
<xml_diff>
--- a/Colpatria.xlsx
+++ b/Colpatria.xlsx
@@ -2319,9 +2319,9 @@
   </sheetPr>
   <dimension ref="A1:AN56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -2463,7 +2463,7 @@
       NETWORKDAYS(J2,L2,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N2" s="28"/>
       <c r="O2" s="28"/>
@@ -2610,7 +2610,7 @@
       NETWORKDAYS(J4,L4,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N4" s="28"/>
       <c r="O4" s="28"/>
@@ -2997,7 +2997,7 @@
       NETWORKDAYS(J9,L9,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N9" s="28"/>
       <c r="O9" s="28"/>
@@ -3678,7 +3678,7 @@
       NETWORKDAYS(J18,L18,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N18" s="55"/>
       <c r="O18" s="55"/>
@@ -4067,7 +4067,7 @@
       NETWORKDAYS(J23,L23,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N23" s="55"/>
       <c r="O23" s="55"/>
@@ -5003,7 +5003,7 @@
       NETWORKDAYS(J35,L35,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N35" s="50"/>
       <c r="O35" s="50"/>
@@ -6257,7 +6257,7 @@
         <v>89</v>
       </c>
       <c r="G52" s="105">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H52" s="24">
         <f>IF(OR(J52="",K52="",K52&lt;J52),0,NETWORKDAYS(J52,K52,Hoja2!$A$2:$A$53))</f>
@@ -6541,7 +6541,7 @@
         <v>89</v>
       </c>
       <c r="G56" s="105">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H56" s="24">
         <f>IF(OR(J56="",K56="",K56&lt;J56),0,NETWORKDAYS(J56,K56,Hoja2!$A$2:$A$53))</f>
@@ -6562,7 +6562,7 @@
       NETWORKDAYS(J56,L56,Hoja2!$A$2:$A$53)
    )
 )</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N56" s="107"/>
       <c r="O56" s="107"/>

</xml_diff>